<commit_message>
updating analysis with new flume load data.
</commit_message>
<xml_diff>
--- a/data/scratch/expandRainSampDates.xlsx
+++ b/data/scratch/expandRainSampDates.xlsx
@@ -15,7 +15,7 @@
     <sheet name="expandRainSampDates" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F152" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K164" sqref="K164"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>